<commit_message>
We have one arcitecture question in TOP MENU block. Basic functions of TOP MENU new status - ALL DONE
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProds\RedBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD72D7FD-97B0-4931-A301-723AD0FFA239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159A2715-CD0B-4FEA-ADB2-ECA5F3FBEB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="3480" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2020" yWindow="3090" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>ФИО</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>Польщиков Владислав Сергеевич</t>
+  </si>
+  <si>
+    <t>Ученики</t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Вид контроля</t>
+  </si>
+  <si>
+    <t>Проверочная работа</t>
+  </si>
+  <si>
+    <t>Тест</t>
+  </si>
+  <si>
+    <t>Ответ у доски</t>
+  </si>
+  <si>
+    <t>Домашняя работа</t>
+  </si>
+  <si>
+    <t>Экзамен</t>
   </si>
 </sst>
 </file>
@@ -120,7 +144,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -128,13 +152,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -415,117 +629,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F2" s="13" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="5">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="5">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="F4" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="5">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="F5" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="5">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="F6" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B7" s="5">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="F7" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="8">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="F8" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All buttons in top menu are DONE. First top menu new status - DONE
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProds\RedBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159A2715-CD0B-4FEA-ADB2-ECA5F3FBEB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1A2E52-75CF-4CFA-A08A-01409DA549BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="3090" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6440" yWindow="2230" windowWidth="16200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>ФИО</t>
   </si>
@@ -115,6 +115,93 @@
   </si>
   <si>
     <t>Экзамен</t>
+  </si>
+  <si>
+    <t>Дисциплина</t>
+  </si>
+  <si>
+    <t>Количество часов</t>
+  </si>
+  <si>
+    <t>Дисциплины</t>
+  </si>
+  <si>
+    <t>Математика (1 класс)</t>
+  </si>
+  <si>
+    <t>Математика (2 класс)</t>
+  </si>
+  <si>
+    <t>Математика (3 класс)</t>
+  </si>
+  <si>
+    <t>Математика (4 класс)</t>
+  </si>
+  <si>
+    <t>Русский язык (1 класс)</t>
+  </si>
+  <si>
+    <t>Русский язык (2 класс)</t>
+  </si>
+  <si>
+    <t>Русский язык (3 класс)</t>
+  </si>
+  <si>
+    <t>Русский язык (4 класс)</t>
+  </si>
+  <si>
+    <t>Классы</t>
+  </si>
+  <si>
+    <t>1А</t>
+  </si>
+  <si>
+    <t>2А</t>
+  </si>
+  <si>
+    <t>3А</t>
+  </si>
+  <si>
+    <t>4А</t>
+  </si>
+  <si>
+    <t>Учителя</t>
+  </si>
+  <si>
+    <t>Аксенов Алексей Владимирович</t>
+  </si>
+  <si>
+    <t>Соколовская Наталья Владимировна</t>
+  </si>
+  <si>
+    <t>Соловьева Татьяна Николаевна</t>
+  </si>
+  <si>
+    <t>semenov11</t>
+  </si>
+  <si>
+    <t>aksenov11</t>
+  </si>
+  <si>
+    <t>solovieva11</t>
+  </si>
+  <si>
+    <t>dima_s</t>
+  </si>
+  <si>
+    <t>lesha_a</t>
+  </si>
+  <si>
+    <t>natasha_s</t>
+  </si>
+  <si>
+    <t>tanya_cs</t>
+  </si>
+  <si>
+    <t>Семенов Дмитрий Алексеевич</t>
+  </si>
+  <si>
+    <t>sokolovskaya11</t>
   </si>
 </sst>
 </file>
@@ -144,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -168,23 +255,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -192,10 +277,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -203,12 +288,42 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -220,98 +335,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -325,30 +348,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -629,150 +650,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="16" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="H1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="H2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1">
         <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="H3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="1">
         <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="H4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="1">
         <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="H5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="1">
         <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="1">
         <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
+      <c r="H7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="3">
         <v>20</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="6"/>
+      <c r="H8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="G12" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1">
+        <v>33</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1">
+        <v>43</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3">
+        <v>29</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>